<commit_message>
fix to secondary source description for E. coli in thresholds, minor edits to news
</commit_message>
<xml_diff>
--- a/inst/extdata/ThresholdMapping.xlsx
+++ b/inst/extdata/ThresholdMapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\MassWateR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D238505-2FFD-4996-ABA0-43A37C0F6474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5E809A-35E2-40C8-9B14-78E5D9CD0D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{178F5C9C-564C-4FDF-AA7C-E06704DA2294}"/>
+    <workbookView xWindow="1290" yWindow="1470" windowWidth="24855" windowHeight="12480" xr2:uid="{178F5C9C-564C-4FDF-AA7C-E06704DA2294}"/>
   </bookViews>
   <sheets>
     <sheet name="Thresholds by uom" sheetId="4" r:id="rId1"/>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="92">
   <si>
     <t>Water Temp</t>
   </si>
@@ -428,6 +428,9 @@
     <t>Based on MassBays review of scientific literature specific to shellfish and salt marsh habitat:
 Boulais M, Chenevert KJ, Demey AT, Darrow ES, Robison MR, Roberts JP, Volety A. Oyster reproduction is compromised by acidification experienced seasonally in coastal regions. Sci Rep. 2017 Oct 16;7(1):13276. doi: 10.1038/s41598-017-13480-3. PMID: 29038546; PMCID: PMC5643346. 
 George G. Waldbusser, Ryan A. Steenson, Mark A. Green "Oyster Shell Dissolution Rates in Estuarine Waters: Effects of pH and Shell Legacy," Journal of Shellfish Research, 30(3), 659-669, (1 December 2011)</t>
+  </si>
+  <si>
+    <t>STV Secondary contact (MADEP)</t>
   </si>
 </sst>
 </file>
@@ -489,24 +492,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -834,981 +836,980 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="27.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="27.5703125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="27.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>0.05</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="E2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <f>C2*1000</f>
         <v>50</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J3" s="3" t="s">
+      <c r="E3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <f>C2*1000/30.97</f>
         <v>1.614465611882467</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>76</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="E4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <f>C2</f>
         <v>0.05</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J5" s="3" t="s">
+      <c r="E5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>5</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>79</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" s="4">
+      <c r="E6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="3">
         <v>5</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" t="s">
         <v>87</v>
       </c>
-      <c r="I6" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J6" s="3" t="s">
+      <c r="I6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <f>C6*1000</f>
         <v>5000</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="4">
+      <c r="E7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="3">
         <f>G6*1000</f>
         <v>5000</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" t="s">
         <v>87</v>
       </c>
-      <c r="I7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J7" s="3" t="s">
+      <c r="I7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>6.5</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>80</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>8.3000000000000007</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>7.5</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" t="s">
         <v>88</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <v>8.5</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>20</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>75</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>28.3</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" t="s">
         <v>74</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <f>(77-32)*5/9</f>
         <v>25</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" t="s">
         <v>64</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="3">
         <v>29.4</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <f>C9*9/5+32</f>
         <v>68</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>75</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <f>ROUND(E9*9/5+32,0)</f>
         <v>83</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" t="s">
         <v>74</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <f>G9*9/5+32</f>
         <v>77</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" t="s">
         <v>64</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="3">
         <f>ROUND(I9*9/5+32,0)</f>
         <v>85</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>70</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" s="4">
+      <c r="E11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="3">
         <v>70</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" t="s">
         <v>73</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="3">
         <v>350</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>85</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <f>C11</f>
         <v>70</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G12" s="4">
+      <c r="E12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="3">
         <f>G11</f>
         <v>70</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" t="s">
         <v>73</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="3">
         <f>I11</f>
         <v>350</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <f>C11</f>
         <v>70</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" s="4">
+      <c r="E13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="3">
         <f>G11</f>
         <v>70</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" t="s">
         <v>73</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="3">
         <f>I11</f>
         <v>350</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J13" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>235</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>73</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>1260</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J14" s="3" t="s">
+      <c r="F14" t="s">
+        <v>91</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>85</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <f>C14</f>
         <v>235</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <f>E14</f>
         <v>1260</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J15" s="3" t="s">
+      <c r="F15" t="s">
+        <v>91</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>86</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <f>C14</f>
         <v>235</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>73</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <f>E14</f>
         <v>1260</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J16" s="3" t="s">
+      <c r="F16" t="s">
+        <v>91</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>230</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <v>860</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G17" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J17" s="3" t="s">
+      <c r="G17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J17" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <f>C17*1000</f>
         <v>230000</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="3">
         <f>E17*1000</f>
         <v>860000</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G18" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J18" s="3" t="s">
+      <c r="G18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>82</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="7">
         <f>C17*1000/35.45</f>
         <v>6488.0112834978836</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" t="s">
         <v>66</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="7">
         <f>E17*1000/35.45</f>
         <v>24259.520451339915</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G19" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J19" s="3" t="s">
+      <c r="G19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>83</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <f>C17</f>
         <v>230</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="3">
         <f>E17</f>
         <v>860</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G20" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J20" s="3" t="s">
+      <c r="G20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J20" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G21" s="4">
+      <c r="C21" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="3">
         <v>0.23300000000000001</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H21" t="s">
         <v>65</v>
       </c>
-      <c r="I21" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J21" s="3" t="s">
+      <c r="I21" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J21" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G22" s="4">
+      <c r="C22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="3">
         <f>G21*1000</f>
         <v>233</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H22" t="s">
         <v>65</v>
       </c>
-      <c r="I22" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J22" s="3" t="s">
+      <c r="I22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J22" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G23" s="8">
+      <c r="C23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G23" s="7">
         <f>G21*1000/14.01</f>
         <v>16.630977872947895</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="H23" t="s">
         <v>65</v>
       </c>
-      <c r="I23" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J23" s="3" t="s">
+      <c r="I23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J23" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G24" s="4">
+      <c r="C24" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G24" s="3">
         <f>G21</f>
         <v>0.23300000000000001</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H24" t="s">
         <v>65</v>
       </c>
-      <c r="I24" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J24" s="3" t="s">
+      <c r="I24" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J24" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G25" s="4">
+      <c r="C25" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G25" s="3">
         <v>0.35</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H25" t="s">
         <v>68</v>
       </c>
-      <c r="I25" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J25" s="3" t="s">
+      <c r="I25" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J25" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G26" s="4">
+      <c r="C26" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G26" s="3">
         <f>G25*1000</f>
         <v>350</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="H26" t="s">
         <v>68</v>
       </c>
-      <c r="I26" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J26" s="3" t="s">
+      <c r="I26" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J26" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G27" s="7">
+      <c r="C27" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G27" s="6">
         <f>G25*1000/14.01</f>
         <v>24.982155603140615</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="H27" t="s">
         <v>68</v>
       </c>
-      <c r="I27" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J27" s="3" t="s">
+      <c r="I27" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J27" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>83</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G28" s="4">
+      <c r="C28" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G28" s="3">
         <f>G25</f>
         <v>0.35</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="H28" t="s">
         <v>68</v>
       </c>
-      <c r="I28" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J28" s="3" t="s">
+      <c r="I28" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J28" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G29" s="4">
+      <c r="C29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G29" s="3">
         <v>5</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="H29" t="s">
         <v>69</v>
       </c>
-      <c r="I29" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J29" s="3" t="s">
+      <c r="I29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J29" s="2" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1832,881 +1833,880 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="27.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="27.5703125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="27.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>0.05</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="E2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>79</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="4">
+      <c r="E3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="3">
         <v>5</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" t="s">
         <v>87</v>
       </c>
-      <c r="I3" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J3" s="3" t="s">
+      <c r="I3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>6.5</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>80</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>8.3000000000000007</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" t="s">
         <v>81</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>7.5</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" t="s">
         <v>88</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>8.5</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>20</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>28.3</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" t="s">
         <v>74</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <f>(77-32)*5/9</f>
         <v>25</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" t="s">
         <v>64</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>29.4</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>70</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" s="4">
+      <c r="E6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="3">
         <v>70</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" t="s">
         <v>73</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
         <v>350</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>235</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>1260</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" t="s">
         <v>72</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J7" s="3" t="s">
+      <c r="G7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>230</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>66</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>860</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J8" s="3" t="s">
+      <c r="G8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" s="4">
+      <c r="C9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="3">
         <v>0.23300000000000001</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" t="s">
         <v>65</v>
       </c>
-      <c r="I9" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J9" s="3" t="s">
+      <c r="I9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="4">
+      <c r="C10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="3">
         <v>0.35</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" t="s">
         <v>68</v>
       </c>
-      <c r="I10" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J10" s="3" t="s">
+      <c r="I10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" s="4">
+      <c r="C11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="3">
         <v>5</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" t="s">
         <v>69</v>
       </c>
-      <c r="I11" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J11" s="3" t="s">
+      <c r="I11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J12" s="3" t="s">
+      <c r="C12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J13" s="3" t="s">
+      <c r="C13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J14" s="3" t="s">
+      <c r="C14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J15" s="3" t="s">
+      <c r="C15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J16" s="3" t="s">
+      <c r="C16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J17" s="3" t="s">
+      <c r="C17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J17" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J18" s="3" t="s">
+      <c r="C18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J19" s="3" t="s">
+      <c r="C19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J20" s="3" t="s">
+      <c r="C20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J20" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J21" s="3" t="s">
+      <c r="C21" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J21" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J22" s="3" t="s">
+      <c r="C22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J22" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J23" s="3" t="s">
+      <c r="C23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J23" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J24" s="3" t="s">
+      <c r="C24" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J24" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I25" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J25" s="3" t="s">
+      <c r="C25" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J25" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J26" s="3" t="s">
+      <c r="C26" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J26" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J27" s="3" t="s">
+      <c r="C27" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J27" s="2" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2729,77 +2729,76 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="5" width="49.140625" style="2" customWidth="1"/>
-    <col min="6" max="11" width="8.7109375" style="2"/>
-    <col min="12" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="5" width="49.140625" style="1" customWidth="1"/>
+    <col min="6" max="11" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="E3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>62</v>
       </c>
       <c r="D4" t="s">
@@ -2808,192 +2807,192 @@
       <c r="E4" t="s">
         <v>90</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="D7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="D8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="B9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="2" t="s">
+      <c r="E9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="B10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" s="2" t="s">
+      <c r="E10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="B11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="2" t="s">
+      <c r="E11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="1" t="s">
         <v>77</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix to thresholdMWR names and column types
</commit_message>
<xml_diff>
--- a/inst/extdata/ThresholdMapping.xlsx
+++ b/inst/extdata/ThresholdMapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\MassWateR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5E809A-35E2-40C8-9B14-78E5D9CD0D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3935785A-4B90-4D08-99DE-B516D624DA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1290" yWindow="1470" windowWidth="24855" windowHeight="12480" xr2:uid="{178F5C9C-564C-4FDF-AA7C-E06704DA2294}"/>
+    <workbookView xWindow="5805" yWindow="3120" windowWidth="24855" windowHeight="12480" xr2:uid="{178F5C9C-564C-4FDF-AA7C-E06704DA2294}"/>
   </bookViews>
   <sheets>
     <sheet name="Thresholds by uom" sheetId="4" r:id="rId1"/>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="94">
   <si>
     <t>Water Temp</t>
   </si>
@@ -431,6 +431,12 @@
   </si>
   <si>
     <t>STV Secondary contact (MADEP)</t>
+  </si>
+  <si>
+    <t>Simple Parameter</t>
+  </si>
+  <si>
+    <t>uom</t>
   </si>
 </sst>
 </file>
@@ -836,7 +842,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="D21" sqref="D21:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,10 +861,10 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>93</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>38</v>
@@ -898,24 +904,12 @@
       <c r="D2" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -931,24 +925,12 @@
       <c r="D3" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -964,24 +946,12 @@
       <c r="D4" t="s">
         <v>76</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -997,24 +967,12 @@
       <c r="D5" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1029,24 +987,16 @@
       <c r="D6" t="s">
         <v>79</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="2"/>
       <c r="G6" s="3">
         <v>5</v>
       </c>
       <c r="H6" t="s">
         <v>87</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1062,12 +1012,8 @@
       <c r="D7" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="2"/>
       <c r="G7" s="3">
         <f>G6*1000</f>
         <v>5000</v>
@@ -1075,12 +1021,8 @@
       <c r="H7" t="s">
         <v>87</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="I7" s="5"/>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1196,12 +1138,8 @@
       <c r="D11" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="2"/>
       <c r="G11" s="3">
         <v>70</v>
       </c>
@@ -1229,12 +1167,8 @@
       <c r="D12" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="2"/>
       <c r="G12" s="3">
         <f>G11</f>
         <v>70</v>
@@ -1264,12 +1198,8 @@
       <c r="D13" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="2"/>
       <c r="G13" s="3">
         <f>G11</f>
         <v>70</v>
@@ -1304,18 +1234,10 @@
       <c r="F14" t="s">
         <v>91</v>
       </c>
-      <c r="G14" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1338,18 +1260,10 @@
       <c r="F15" t="s">
         <v>91</v>
       </c>
-      <c r="G15" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1372,18 +1286,10 @@
       <c r="F16" t="s">
         <v>91</v>
       </c>
-      <c r="G16" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1404,18 +1310,10 @@
       <c r="F17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G17" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -1438,18 +1336,10 @@
       <c r="F18" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G18" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="G18" s="5"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1472,18 +1362,10 @@
       <c r="F19" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G19" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="G19" s="5"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -1506,18 +1388,10 @@
       <c r="F20" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G20" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -1526,30 +1400,18 @@
       <c r="B21" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="2"/>
       <c r="G21" s="3">
         <v>0.23300000000000001</v>
       </c>
       <c r="H21" t="s">
         <v>65</v>
       </c>
-      <c r="I21" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="I21" s="5"/>
+      <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -1558,18 +1420,10 @@
       <c r="B22" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="2"/>
       <c r="G22" s="3">
         <f>G21*1000</f>
         <v>233</v>
@@ -1577,12 +1431,8 @@
       <c r="H22" t="s">
         <v>65</v>
       </c>
-      <c r="I22" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="I22" s="5"/>
+      <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1591,18 +1441,10 @@
       <c r="B23" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="2"/>
       <c r="G23" s="7">
         <f>G21*1000/14.01</f>
         <v>16.630977872947895</v>
@@ -1610,12 +1452,8 @@
       <c r="H23" t="s">
         <v>65</v>
       </c>
-      <c r="I23" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="I23" s="5"/>
+      <c r="J23" s="2"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -1624,18 +1462,10 @@
       <c r="B24" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="2"/>
       <c r="G24" s="3">
         <f>G21</f>
         <v>0.23300000000000001</v>
@@ -1643,12 +1473,8 @@
       <c r="H24" t="s">
         <v>65</v>
       </c>
-      <c r="I24" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="I24" s="5"/>
+      <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1657,30 +1483,18 @@
       <c r="B25" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="2"/>
       <c r="G25" s="3">
         <v>0.35</v>
       </c>
       <c r="H25" t="s">
         <v>68</v>
       </c>
-      <c r="I25" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="I25" s="5"/>
+      <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1689,18 +1503,10 @@
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="2"/>
       <c r="G26" s="3">
         <f>G25*1000</f>
         <v>350</v>
@@ -1708,12 +1514,8 @@
       <c r="H26" t="s">
         <v>68</v>
       </c>
-      <c r="I26" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="I26" s="5"/>
+      <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -1722,18 +1524,10 @@
       <c r="B27" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="2"/>
       <c r="G27" s="6">
         <f>G25*1000/14.01</f>
         <v>24.982155603140615</v>
@@ -1741,12 +1535,8 @@
       <c r="H27" t="s">
         <v>68</v>
       </c>
-      <c r="I27" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="I27" s="5"/>
+      <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -1755,18 +1545,10 @@
       <c r="B28" t="s">
         <v>83</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="2"/>
       <c r="G28" s="3">
         <f>G25</f>
         <v>0.35</v>
@@ -1774,12 +1556,8 @@
       <c r="H28" t="s">
         <v>68</v>
       </c>
-      <c r="I28" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="I28" s="5"/>
+      <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -1788,30 +1566,18 @@
       <c r="B29" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="2"/>
       <c r="G29" s="3">
         <v>5</v>
       </c>
       <c r="H29" t="s">
         <v>69</v>
       </c>
-      <c r="I29" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="I29" s="5"/>
+      <c r="J29" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update thresholdMWR for Enterococcus secondary label correct
</commit_message>
<xml_diff>
--- a/inst/extdata/ThresholdMapping.xlsx
+++ b/inst/extdata/ThresholdMapping.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\MassWateR\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbeck\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3935785A-4B90-4D08-99DE-B516D624DA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FD8F5A-A70C-42FB-9DCE-517BB2AD9F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5805" yWindow="3120" windowWidth="24855" windowHeight="12480" xr2:uid="{178F5C9C-564C-4FDF-AA7C-E06704DA2294}"/>
+    <workbookView xWindow="34920" yWindow="3120" windowWidth="17280" windowHeight="8880" xr2:uid="{178F5C9C-564C-4FDF-AA7C-E06704DA2294}"/>
   </bookViews>
   <sheets>
     <sheet name="Thresholds by uom" sheetId="4" r:id="rId1"/>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="93">
   <si>
     <t>Water Temp</t>
   </si>
@@ -369,9 +369,6 @@
   </si>
   <si>
     <t>Class SA/SB/SC (MADEP)</t>
-  </si>
-  <si>
-    <t>STV Secondary contact (EPA)</t>
   </si>
   <si>
     <t>BAV Primary contact (EPA)</t>
@@ -839,32 +836,32 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D21" sqref="D21:D29"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="27.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="27.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="27.5546875" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="27.5546875" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="27.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
         <v>92</v>
-      </c>
-      <c r="B1" t="s">
-        <v>93</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>38</v>
@@ -891,7 +888,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -902,16 +899,28 @@
         <v>0.05</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -923,58 +932,94 @@
         <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" s="6">
         <f>C2*1000/30.97</f>
         <v>1.614465611882467</v>
       </c>
       <c r="D4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5" s="3">
         <f>C2</f>
         <v>0.05</v>
       </c>
       <c r="D5" t="s">
-        <v>76</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -985,20 +1030,28 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="2"/>
+        <v>78</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="G6" s="3">
         <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>87</v>
-      </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1010,21 +1063,29 @@
         <v>5000</v>
       </c>
       <c r="D7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="2"/>
+        <v>78</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="G7" s="3">
         <f>G6*1000</f>
         <v>5000</v>
       </c>
       <c r="H7" t="s">
-        <v>87</v>
-      </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1035,28 +1096,28 @@
         <v>6.5</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E8" s="3">
         <v>8.3000000000000007</v>
       </c>
       <c r="F8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G8" s="3">
         <v>7.5</v>
       </c>
       <c r="H8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I8" s="3">
         <v>8.5</v>
       </c>
       <c r="J8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1067,13 +1128,13 @@
         <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E9" s="3">
         <v>28.3</v>
       </c>
       <c r="F9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G9" s="3">
         <f>(77-32)*5/9</f>
@@ -1089,26 +1150,26 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" s="3">
         <f>C9*9/5+32</f>
         <v>68</v>
       </c>
       <c r="D10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E10" s="3">
         <f>ROUND(E9*9/5+32,0)</f>
         <v>83</v>
       </c>
       <c r="F10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G10" s="3">
         <f>G9*9/5+32</f>
@@ -1125,7 +1186,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1136,86 +1197,98 @@
         <v>70</v>
       </c>
       <c r="D11" t="s">
-        <v>73</v>
-      </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="G11" s="3">
         <v>70</v>
       </c>
       <c r="H11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I11" s="3">
         <v>350</v>
       </c>
       <c r="J11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C12" s="3">
         <f>C11</f>
         <v>70</v>
       </c>
       <c r="D12" t="s">
-        <v>73</v>
-      </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="G12" s="3">
         <f>G11</f>
         <v>70</v>
       </c>
       <c r="H12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I12" s="3">
         <f>I11</f>
         <v>350</v>
       </c>
       <c r="J12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C13" s="3">
         <f>C11</f>
         <v>70</v>
       </c>
       <c r="D13" t="s">
-        <v>73</v>
-      </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="G13" s="3">
         <f>G11</f>
         <v>70</v>
       </c>
       <c r="H13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I13" s="3">
         <f>I11</f>
         <v>350</v>
       </c>
       <c r="J13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1226,72 +1299,96 @@
         <v>235</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E14" s="3">
         <v>1260</v>
       </c>
       <c r="F14" t="s">
-        <v>91</v>
-      </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C15" s="3">
         <f>C14</f>
         <v>235</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E15" s="3">
         <f>E14</f>
         <v>1260</v>
       </c>
       <c r="F15" t="s">
-        <v>91</v>
-      </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C16" s="3">
         <f>C14</f>
         <v>235</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E16" s="3">
         <f>E14</f>
         <v>1260</v>
       </c>
       <c r="F16" t="s">
-        <v>91</v>
-      </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1310,12 +1407,20 @@
       <c r="F17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1336,17 +1441,25 @@
       <c r="F18" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C19" s="7">
         <f>C17*1000/35.45</f>
@@ -1362,17 +1475,25 @@
       <c r="F19" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C20" s="3">
         <f>C17</f>
@@ -1388,42 +1509,70 @@
       <c r="F20" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>17</v>
       </c>
       <c r="B21" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="2"/>
+      <c r="C21" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="G21" s="3">
         <v>0.23300000000000001</v>
       </c>
       <c r="H21" t="s">
         <v>65</v>
       </c>
-      <c r="I21" s="5"/>
-      <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I21" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
       <c r="B22" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="2"/>
+      <c r="C22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="G22" s="3">
         <f>G21*1000</f>
         <v>233</v>
@@ -1431,20 +1580,32 @@
       <c r="H22" t="s">
         <v>65</v>
       </c>
-      <c r="I22" s="5"/>
-      <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="2"/>
+        <v>81</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="G23" s="7">
         <f>G21*1000/14.01</f>
         <v>16.630977872947895</v>
@@ -1452,20 +1613,32 @@
       <c r="H23" t="s">
         <v>65</v>
       </c>
-      <c r="I23" s="5"/>
-      <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="2"/>
+        <v>82</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="G24" s="3">
         <f>G21</f>
         <v>0.23300000000000001</v>
@@ -1473,40 +1646,64 @@
       <c r="H24" t="s">
         <v>65</v>
       </c>
-      <c r="I24" s="5"/>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I24" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>16</v>
       </c>
       <c r="B25" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="2"/>
+      <c r="C25" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="G25" s="3">
         <v>0.35</v>
       </c>
       <c r="H25" t="s">
         <v>68</v>
       </c>
-      <c r="I25" s="5"/>
-      <c r="J25" s="2"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I25" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>16</v>
       </c>
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="2"/>
+      <c r="C26" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="G26" s="3">
         <f>G25*1000</f>
         <v>350</v>
@@ -1514,20 +1711,32 @@
       <c r="H26" t="s">
         <v>68</v>
       </c>
-      <c r="I26" s="5"/>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I26" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="2"/>
+        <v>81</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="G27" s="6">
         <f>G25*1000/14.01</f>
         <v>24.982155603140615</v>
@@ -1535,20 +1744,32 @@
       <c r="H27" t="s">
         <v>68</v>
       </c>
-      <c r="I27" s="5"/>
-      <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I27" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>83</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="2"/>
+        <v>82</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="G28" s="3">
         <f>G25</f>
         <v>0.35</v>
@@ -1556,28 +1777,44 @@
       <c r="H28" t="s">
         <v>68</v>
       </c>
-      <c r="I28" s="5"/>
-      <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I28" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>11</v>
       </c>
       <c r="B29" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="2"/>
+      <c r="C29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="G29" s="3">
         <v>5</v>
       </c>
       <c r="H29" t="s">
         <v>69</v>
       </c>
-      <c r="I29" s="5"/>
-      <c r="J29" s="2"/>
+      <c r="I29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1594,24 +1831,24 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="27.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="27.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="27.5546875" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="27.5546875" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="27.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -1643,7 +1880,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1654,7 +1891,7 @@
         <v>0.05</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>53</v>
@@ -1675,7 +1912,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1686,7 +1923,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>53</v>
@@ -1698,7 +1935,7 @@
         <v>5</v>
       </c>
       <c r="H3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>53</v>
@@ -1707,7 +1944,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1718,28 +1955,28 @@
         <v>6.5</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E4" s="3">
         <v>8.3000000000000007</v>
       </c>
       <c r="F4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G4" s="3">
         <v>7.5</v>
       </c>
       <c r="H4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I4" s="3">
         <v>8.5</v>
       </c>
       <c r="J4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1750,13 +1987,13 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E5" s="3">
         <v>28.3</v>
       </c>
       <c r="F5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G5" s="3">
         <f>(77-32)*5/9</f>
@@ -1772,7 +2009,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1783,7 +2020,7 @@
         <v>70</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>53</v>
@@ -1795,16 +2032,16 @@
         <v>70</v>
       </c>
       <c r="H6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I6" s="3">
         <v>350</v>
       </c>
       <c r="J6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1815,13 +2052,13 @@
         <v>235</v>
       </c>
       <c r="D7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E7" s="3">
         <v>1260</v>
       </c>
       <c r="F7" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>53</v>
@@ -1836,7 +2073,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1868,7 +2105,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1900,7 +2137,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1932,7 +2169,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1964,7 +2201,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1996,7 +2233,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -2028,7 +2265,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -2060,7 +2297,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -2092,7 +2329,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -2124,7 +2361,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -2156,7 +2393,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -2188,7 +2425,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2220,7 +2457,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -2252,7 +2489,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -2284,7 +2521,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -2316,7 +2553,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -2348,7 +2585,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -2380,7 +2617,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2412,7 +2649,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -2444,7 +2681,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -2490,17 +2727,17 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="5" width="49.140625" style="1" customWidth="1"/>
-    <col min="6" max="11" width="8.7109375" style="1"/>
+    <col min="2" max="5" width="49.21875" style="1" customWidth="1"/>
+    <col min="6" max="11" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -2517,12 +2754,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>53</v>
@@ -2534,10 +2771,10 @@
         <v>53</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2554,10 +2791,10 @@
         <v>53</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -2568,16 +2805,16 @@
         <v>62</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -2594,10 +2831,10 @@
         <v>63</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2614,10 +2851,10 @@
         <v>60</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -2634,10 +2871,10 @@
         <v>53</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2654,10 +2891,10 @@
         <v>53</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -2674,10 +2911,10 @@
         <v>53</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2694,10 +2931,10 @@
         <v>53</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -2714,52 +2951,52 @@
         <v>53</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F12" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F13" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F14" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F15" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F16" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F17" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F18" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F19" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F20" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>